<commit_message>
Create graphs for thesis
</commit_message>
<xml_diff>
--- a/pomiary/krok.xlsx
+++ b/pomiary/krok.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\arduinko\inzynierka\pomiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC49C805-DF15-4615-9D16-1C0C3AD248C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B7682-A8DD-49DA-B73E-A01BA030DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
   <si>
     <t>C</t>
   </si>
@@ -52,9 +54,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>nNodes</t>
-  </si>
-  <si>
     <t>Inputs</t>
   </si>
   <si>
@@ -98,6 +97,9 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>nElements</t>
   </si>
 </sst>
 </file>
@@ -421,26 +423,26 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -448,27 +450,27 @@
         <v>700</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <f xml:space="preserve"> 1.5*B6 - 0.5*B7</f>
-        <v>1.75E-3</v>
+        <f xml:space="preserve"> (B6 + B7)/2</f>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2">
         <f>_xlfn.FLOOR.MATH(F3/F6 + 1)</f>
-        <v>354</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -476,41 +478,41 @@
         <v>7800</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <f>F2/B5</f>
-        <v>8.7499999999999994E-2</v>
+        <f>B5/F2</f>
+        <v>8.8888888888888875</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <f>B8/(B9+1)</f>
-        <v>2.380952380952381E-5</v>
+        <v>7.2727272727272734E-4</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -518,17 +520,17 @@
         <v>0.02</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <f>B4/(B2*B3)</f>
         <v>4.5787545787545788E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -536,20 +538,20 @@
         <v>2E-3</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <f>(F4^2)/(0.5*F5)</f>
-        <v>2.4761904761904762E-4</v>
+        <v>0.23103471074380169</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -557,26 +559,372 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>5.0000000000000001E-4</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461CF43E-73F3-43A9-88FB-B72CD12F4AD8}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>700</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <f xml:space="preserve"> (B6 + B7)/2</f>
+        <v>5.2499999999999995E-3</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <f>_xlfn.FLOOR.MATH(F3/F6 + 1)</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f>B5/F2</f>
+        <v>3.8095238095238102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>B8/(B9+1)</f>
+        <v>1.5625E-4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <f>B4/(B2*B3)</f>
+        <v>4.5787545787545788E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <f>(F4^2)/(0.5*F5)</f>
+        <v>1.06640625E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FCC528-6AA3-4799-902F-468FB6F2D1F8}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>700</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <f xml:space="preserve"> (B6 + B7)/2</f>
+        <v>5.2499999999999995E-3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <f>_xlfn.FLOOR.MATH(F3/F6 + 1)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f>B5/F2</f>
+        <v>3.8095238095238102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>B8/(B9+1)</f>
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <f>B4/(B2*B3)</f>
+        <v>4.5787545787545788E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <f>(F4^2)/(0.5*F5)</f>
+        <v>0.3033333333333334</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
       <c r="B9">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add dtau to tables, add long heating graph
</commit_message>
<xml_diff>
--- a/pomiary/krok.xlsx
+++ b/pomiary/krok.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\arduinko\inzynierka\pomiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B7682-A8DD-49DA-B73E-A01BA030DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F351EC78-F2BB-434A-894C-E37C9AE47EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
+    <sheet name="testowy" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="22">
   <si>
     <t>C</t>
   </si>
@@ -422,16 +423,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -442,7 +443,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,7 +471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -491,7 +492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -512,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -530,7 +531,7 @@
         <v>4.5787545787545788E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -551,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -562,7 +563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -573,7 +574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -595,16 +596,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461CF43E-73F3-43A9-88FB-B72CD12F4AD8}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -615,7 +616,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +644,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -664,7 +665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -685,7 +686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -703,7 +704,7 @@
         <v>4.5787545787545788E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -724,7 +725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -735,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -746,7 +747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -768,16 +769,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FCC528-6AA3-4799-902F-468FB6F2D1F8}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -788,7 +789,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -816,7 +817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -837,7 +838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -858,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -876,7 +877,7 @@
         <v>4.5787545787545788E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -897,7 +898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -908,7 +909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -919,12 +920,185 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DCDA2D-33BB-4993-9547-38669567BB09}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>700</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <f xml:space="preserve"> (B6 + B7)/2</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <f>_xlfn.FLOOR.MATH(F3/F6 + 1)</f>
+        <v>866</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f>B5/F2</f>
+        <v>200</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>B8/(B9+1)</f>
+        <v>7.2727272727272734E-4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <f>B4/(B2*B3)</f>
+        <v>4.5787545787545788E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1E-4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <f>(F4^2)/(0.5*F5)</f>
+        <v>0.23103471074380169</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1E-4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>